<commit_message>
:zap: spacecraft results + charts updated
</commit_message>
<xml_diff>
--- a/Execucoes Gerais/novo_final_AGEO2-vs-AGEOsvar.xlsx
+++ b/Execucoes Gerais/novo_final_AGEO2-vs-AGEOsvar.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="14460" windowHeight="7905" activeTab="2"/>
+    <workbookView windowWidth="14460" windowHeight="7860" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="GRI" sheetId="7" r:id="rId1"/>
@@ -80,10 +80,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -94,9 +94,47 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -111,24 +149,62 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -149,52 +225,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -202,37 +232,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -247,19 +247,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -271,19 +259,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -295,25 +283,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -331,7 +331,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -343,91 +427,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -446,6 +446,71 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -473,218 +538,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1138,7 +1138,9 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="0070C0"/>
+                <a:srgbClr val="70AD47">
+                  <a:lumMod val="75000"/>
+                </a:srgbClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1149,11 +1151,15 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="0070C0"/>
+                <a:srgbClr val="70AD47">
+                  <a:lumMod val="75000"/>
+                </a:srgbClr>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:srgbClr val="0070C0"/>
+                  <a:srgbClr val="70AD47">
+                    <a:lumMod val="75000"/>
+                  </a:srgbClr>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -1433,22 +1439,22 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="0070C0"/>
+                <a:srgbClr val="ED7D31"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="triangle"/>
+            <c:symbol val="circle"/>
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="0070C0"/>
+                <a:srgbClr val="ED7D31"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:srgbClr val="0070C0"/>
+                  <a:srgbClr val="ED7D31"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -1748,7 +1754,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pt-PT" altLang="en-US"/>
-                  <a:t>NFE</a:t>
+                  <a:t>Número de avaliações da função objetivo</a:t>
                 </a:r>
                 <a:endParaRPr lang="pt-PT" altLang="en-US"/>
               </a:p>
@@ -1758,8 +1764,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.521536243298832"/>
-              <c:y val="0.916674844831117"/>
+              <c:x val="0.260956790123457"/>
+              <c:y val="0.921064814814815"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -2353,7 +2359,9 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="0070C0"/>
+                <a:srgbClr val="70AD47">
+                  <a:lumMod val="75000"/>
+                </a:srgbClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -2364,11 +2372,15 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="0070C0"/>
+                <a:srgbClr val="70AD47">
+                  <a:lumMod val="75000"/>
+                </a:srgbClr>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:srgbClr val="0070C0"/>
+                  <a:srgbClr val="70AD47">
+                    <a:lumMod val="75000"/>
+                  </a:srgbClr>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -2648,22 +2660,22 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="0070C0"/>
+                <a:srgbClr val="ED7D31"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="triangle"/>
+            <c:symbol val="circle"/>
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="0070C0"/>
+                <a:srgbClr val="ED7D31"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:srgbClr val="0070C0"/>
+                  <a:srgbClr val="ED7D31"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -2963,7 +2975,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pt-PT" altLang="en-US"/>
-                  <a:t>NFE</a:t>
+                  <a:t>Número de avaliações da função objetivo</a:t>
                 </a:r>
                 <a:endParaRPr lang="pt-PT" altLang="en-US"/>
               </a:p>
@@ -2973,8 +2985,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.521536243298832"/>
-              <c:y val="0.916674844831117"/>
+              <c:x val="0.258641975308642"/>
+              <c:y val="0.91412037037037"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -3569,7 +3581,9 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="0070C0"/>
+                <a:srgbClr val="70AD47">
+                  <a:lumMod val="75000"/>
+                </a:srgbClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -3580,11 +3594,15 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="0070C0"/>
+                <a:srgbClr val="70AD47">
+                  <a:lumMod val="75000"/>
+                </a:srgbClr>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:srgbClr val="0070C0"/>
+                  <a:srgbClr val="70AD47">
+                    <a:lumMod val="75000"/>
+                  </a:srgbClr>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -3864,22 +3882,22 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="0070C0"/>
+                <a:srgbClr val="ED7D31"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="triangle"/>
+            <c:symbol val="circle"/>
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="0070C0"/>
+                <a:srgbClr val="ED7D31"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:srgbClr val="0070C0"/>
+                  <a:srgbClr val="ED7D31"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -4179,7 +4197,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pt-PT" altLang="en-US"/>
-                  <a:t>NFE</a:t>
+                  <a:t>Número de avaliações da função objetivo</a:t>
                 </a:r>
                 <a:endParaRPr lang="pt-PT" altLang="en-US"/>
               </a:p>
@@ -4189,8 +4207,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.521536243298832"/>
-              <c:y val="0.916674844831117"/>
+              <c:x val="0.25992277992278"/>
+              <c:y val="0.913666281998439"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -4783,7 +4801,9 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="0070C0"/>
+                <a:srgbClr val="70AD47">
+                  <a:lumMod val="75000"/>
+                </a:srgbClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -4794,11 +4814,15 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="0070C0"/>
+                <a:srgbClr val="70AD47">
+                  <a:lumMod val="75000"/>
+                </a:srgbClr>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:srgbClr val="0070C0"/>
+                  <a:srgbClr val="70AD47">
+                    <a:lumMod val="75000"/>
+                  </a:srgbClr>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -5078,22 +5102,22 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="0070C0"/>
+                <a:srgbClr val="ED7D31"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="triangle"/>
+            <c:symbol val="circle"/>
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="0070C0"/>
+                <a:srgbClr val="ED7D31"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:srgbClr val="0070C0"/>
+                  <a:srgbClr val="ED7D31"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -5393,7 +5417,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pt-PT" altLang="en-US"/>
-                  <a:t>NFE</a:t>
+                  <a:t>Número de avaliações da função objetivo</a:t>
                 </a:r>
                 <a:endParaRPr lang="pt-PT" altLang="en-US"/>
               </a:p>
@@ -5403,8 +5427,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.521536243298832"/>
-              <c:y val="0.916674844831117"/>
+              <c:x val="0.249382716049383"/>
+              <c:y val="0.91412037037037"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -5998,7 +6022,9 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="0070C0"/>
+                <a:srgbClr val="70AD47">
+                  <a:lumMod val="75000"/>
+                </a:srgbClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -6009,11 +6035,15 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="0070C0"/>
+                <a:srgbClr val="70AD47">
+                  <a:lumMod val="50000"/>
+                </a:srgbClr>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:srgbClr val="0070C0"/>
+                  <a:srgbClr val="70AD47">
+                    <a:lumMod val="75000"/>
+                  </a:srgbClr>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -6293,22 +6323,22 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="0070C0"/>
+                <a:srgbClr val="ED7D31"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="triangle"/>
+            <c:symbol val="circle"/>
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="0070C0"/>
+                <a:srgbClr val="ED7D31"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:srgbClr val="0070C0"/>
+                  <a:srgbClr val="ED7D31"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -6608,7 +6638,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pt-PT" altLang="en-US"/>
-                  <a:t>NFE</a:t>
+                  <a:t>Número de avaliações da função objetivo</a:t>
                 </a:r>
                 <a:endParaRPr lang="pt-PT" altLang="en-US"/>
               </a:p>
@@ -6618,8 +6648,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.521536243298832"/>
-              <c:y val="0.916674844831117"/>
+              <c:x val="0.254012345679012"/>
+              <c:y val="0.920147067053339"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -7212,7 +7242,9 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="0070C0"/>
+                <a:srgbClr val="70AD47">
+                  <a:lumMod val="75000"/>
+                </a:srgbClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -7223,11 +7255,15 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="0070C0"/>
+                <a:srgbClr val="70AD47">
+                  <a:lumMod val="75000"/>
+                </a:srgbClr>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:srgbClr val="0070C0"/>
+                  <a:srgbClr val="70AD47">
+                    <a:lumMod val="75000"/>
+                  </a:srgbClr>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -7507,22 +7543,22 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="0070C0"/>
+                <a:srgbClr val="ED7D31"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="triangle"/>
+            <c:symbol val="circle"/>
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="0070C0"/>
+                <a:srgbClr val="ED7D31"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:srgbClr val="0070C0"/>
+                  <a:srgbClr val="ED7D31"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -7822,7 +7858,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pt-PT" altLang="en-US"/>
-                  <a:t>NFE</a:t>
+                  <a:t>Número de avaliações da função objetivo</a:t>
                 </a:r>
                 <a:endParaRPr lang="pt-PT" altLang="en-US"/>
               </a:p>
@@ -7832,7 +7868,7 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.521536243298832"/>
+              <c:x val="0.254012345679012"/>
               <c:y val="0.916674844831117"/>
             </c:manualLayout>
           </c:layout>
@@ -11458,13 +11494,13 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>3175</xdr:rowOff>
+      <xdr:rowOff>2540</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
       <xdr:row>56</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
+      <xdr:rowOff>11430</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -11472,8 +11508,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="685800" y="7423150"/>
-        <a:ext cx="4114800" cy="2743200"/>
+        <a:off x="685800" y="7422515"/>
+        <a:ext cx="4114800" cy="2723515"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -13364,7 +13400,7 @@
   <dimension ref="A1:D68"/>
   <sheetViews>
     <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A66" sqref="A61:A66"/>
+      <selection activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="3"/>
@@ -14044,1366 +14080,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:D66"/>
-  <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61:A66"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="3"/>
-  <cols>
-    <col min="2" max="5" width="12.625"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2">
-        <v>5</v>
-      </c>
-      <c r="B2">
-        <v>222.161129866036</v>
-      </c>
-      <c r="C2">
-        <v>222.161129866036</v>
-      </c>
-      <c r="D2">
-        <v>222.161129866036</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3">
-        <v>50</v>
-      </c>
-      <c r="B3">
-        <v>213.724838821676</v>
-      </c>
-      <c r="C3">
-        <v>213.724838821676</v>
-      </c>
-      <c r="D3">
-        <v>213.724838821676</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4">
-        <v>100</v>
-      </c>
-      <c r="B4">
-        <v>211.685872228184</v>
-      </c>
-      <c r="C4">
-        <v>211.685872228184</v>
-      </c>
-      <c r="D4">
-        <v>211.685872228184</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5">
-        <v>500</v>
-      </c>
-      <c r="B5">
-        <v>204.515499401897</v>
-      </c>
-      <c r="C5">
-        <v>149.449777442719</v>
-      </c>
-      <c r="D5">
-        <v>172.267340865898</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6">
-        <v>1000</v>
-      </c>
-      <c r="B6">
-        <v>184.750695749215</v>
-      </c>
-      <c r="C6">
-        <v>80.663463015223</v>
-      </c>
-      <c r="D6">
-        <v>98.2744348587591</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7">
-        <v>1500</v>
-      </c>
-      <c r="B7">
-        <v>164.465094624622</v>
-      </c>
-      <c r="C7">
-        <v>55.5958350050346</v>
-      </c>
-      <c r="D7">
-        <v>60.9599290430378</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8">
-        <v>2000</v>
-      </c>
-      <c r="B8">
-        <v>138.575992131484</v>
-      </c>
-      <c r="C8">
-        <v>40.7587350167379</v>
-      </c>
-      <c r="D8">
-        <v>35.0600721878919</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9">
-        <v>2500</v>
-      </c>
-      <c r="B9">
-        <v>119.922287280342</v>
-      </c>
-      <c r="C9">
-        <v>37.2310478129347</v>
-      </c>
-      <c r="D9">
-        <v>28.4665142296936</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10">
-        <v>3000</v>
-      </c>
-      <c r="B10">
-        <v>97.9407311838834</v>
-      </c>
-      <c r="C10">
-        <v>35.8153540633938</v>
-      </c>
-      <c r="D10">
-        <v>23.894178092588</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11">
-        <v>3500</v>
-      </c>
-      <c r="B11">
-        <v>87.7959498851028</v>
-      </c>
-      <c r="C11">
-        <v>34.5709190485729</v>
-      </c>
-      <c r="D11">
-        <v>23.6504376355184</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12">
-        <v>4000</v>
-      </c>
-      <c r="B12">
-        <v>73.4884609402364</v>
-      </c>
-      <c r="C12">
-        <v>33.1898609925408</v>
-      </c>
-      <c r="D12">
-        <v>23.0969328230867</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13">
-        <v>4500</v>
-      </c>
-      <c r="B13">
-        <v>65.0233974426678</v>
-      </c>
-      <c r="C13">
-        <v>32.8577532110956</v>
-      </c>
-      <c r="D13">
-        <v>23.006663331618</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14">
-        <v>5000</v>
-      </c>
-      <c r="B14">
-        <v>57.3025687064767</v>
-      </c>
-      <c r="C14">
-        <v>32.4111113053343</v>
-      </c>
-      <c r="D14">
-        <v>22.9883156411679</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15">
-        <v>6000</v>
-      </c>
-      <c r="B15">
-        <v>46.1653576900982</v>
-      </c>
-      <c r="C15">
-        <v>32.1101767449222</v>
-      </c>
-      <c r="D15">
-        <v>22.9830527697315</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16">
-        <v>7000</v>
-      </c>
-      <c r="B16">
-        <v>38.1521149027307</v>
-      </c>
-      <c r="C16">
-        <v>31.8996822561839</v>
-      </c>
-      <c r="D16">
-        <v>22.9830275566717</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17">
-        <v>8000</v>
-      </c>
-      <c r="B17">
-        <v>32.2688119830113</v>
-      </c>
-      <c r="C17">
-        <v>31.5867922309758</v>
-      </c>
-      <c r="D17">
-        <v>22.982949079113</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18">
-        <v>9000</v>
-      </c>
-      <c r="B18">
-        <v>27.7597428378178</v>
-      </c>
-      <c r="C18">
-        <v>31.133469335833</v>
-      </c>
-      <c r="D18">
-        <v>22.9829477488005</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19">
-        <v>10000</v>
-      </c>
-      <c r="B19">
-        <v>24.9656141777948</v>
-      </c>
-      <c r="C19">
-        <v>31.133469335833</v>
-      </c>
-      <c r="D19">
-        <v>22.9829477488005</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20">
-        <v>12000</v>
-      </c>
-      <c r="B20">
-        <v>21.9647140986413</v>
-      </c>
-      <c r="C20">
-        <v>31.0993392553022</v>
-      </c>
-      <c r="D20">
-        <v>22.9829477488005</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21">
-        <v>14000</v>
-      </c>
-      <c r="B21">
-        <v>20.7589879315573</v>
-      </c>
-      <c r="C21">
-        <v>30.963941267577</v>
-      </c>
-      <c r="D21">
-        <v>22.9829477488005</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22">
-        <v>16000</v>
-      </c>
-      <c r="B22">
-        <v>20.320069303179</v>
-      </c>
-      <c r="C22">
-        <v>30.8132192429305</v>
-      </c>
-      <c r="D22">
-        <v>22.9829477488005</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23">
-        <v>18000</v>
-      </c>
-      <c r="B23">
-        <v>20.1162173990172</v>
-      </c>
-      <c r="C23">
-        <v>30.8132192429305</v>
-      </c>
-      <c r="D23">
-        <v>22.9829477488005</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24">
-        <v>20000</v>
-      </c>
-      <c r="B24">
-        <v>19.9195687017421</v>
-      </c>
-      <c r="C24">
-        <v>30.444225290351</v>
-      </c>
-      <c r="D24">
-        <v>22.9829477488005</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25">
-        <v>25000</v>
-      </c>
-      <c r="B25">
-        <v>19.8540728752238</v>
-      </c>
-      <c r="C25">
-        <v>30.444225290351</v>
-      </c>
-      <c r="D25">
-        <v>22.9829477488005</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26">
-        <v>30000</v>
-      </c>
-      <c r="B26">
-        <v>19.8428338080667</v>
-      </c>
-      <c r="C26">
-        <v>30.2103916561594</v>
-      </c>
-      <c r="D26">
-        <v>22.9829477488005</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27">
-        <v>35000</v>
-      </c>
-      <c r="B27">
-        <v>19.8141065956705</v>
-      </c>
-      <c r="C27">
-        <v>30.2103916561594</v>
-      </c>
-      <c r="D27">
-        <v>22.9829477488005</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28">
-        <v>40000</v>
-      </c>
-      <c r="B28">
-        <v>19.7453584808793</v>
-      </c>
-      <c r="C28">
-        <v>29.8394041069721</v>
-      </c>
-      <c r="D28">
-        <v>22.9829477488005</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29">
-        <v>45000</v>
-      </c>
-      <c r="B29">
-        <v>18.983288489317</v>
-      </c>
-      <c r="C29">
-        <v>28.9133601927686</v>
-      </c>
-      <c r="D29">
-        <v>22.9829477488005</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30">
-        <v>50000</v>
-      </c>
-      <c r="B30">
-        <v>18.4746244124938</v>
-      </c>
-      <c r="C30">
-        <v>28.9133601927686</v>
-      </c>
-      <c r="D30">
-        <v>22.9829477488005</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31">
-        <v>55000</v>
-      </c>
-      <c r="B31">
-        <v>17.9927469397173</v>
-      </c>
-      <c r="C31">
-        <v>28.9133601927686</v>
-      </c>
-      <c r="D31">
-        <v>22.9829477488005</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32">
-        <v>60000</v>
-      </c>
-      <c r="B32">
-        <v>17.695699611482</v>
-      </c>
-      <c r="C32">
-        <v>28.9133601927686</v>
-      </c>
-      <c r="D32">
-        <v>22.9829477488005</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33">
-        <v>65000</v>
-      </c>
-      <c r="B33">
-        <v>17.4420595328849</v>
-      </c>
-      <c r="C33">
-        <v>28.9133601927686</v>
-      </c>
-      <c r="D33">
-        <v>22.9829477488005</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34">
-        <v>70000</v>
-      </c>
-      <c r="B34">
-        <v>17.2169735857428</v>
-      </c>
-      <c r="C34">
-        <v>28.9133601927686</v>
-      </c>
-      <c r="D34">
-        <v>22.9829477488005</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35">
-        <v>75000</v>
-      </c>
-      <c r="B35">
-        <v>16.9728026776156</v>
-      </c>
-      <c r="C35">
-        <v>28.9133601927686</v>
-      </c>
-      <c r="D35">
-        <v>22.9829477488005</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36">
-        <v>80000</v>
-      </c>
-      <c r="B36">
-        <v>16.8804150028953</v>
-      </c>
-      <c r="C36">
-        <v>28.9133601927686</v>
-      </c>
-      <c r="D36">
-        <v>22.9829477488005</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37">
-        <v>85000</v>
-      </c>
-      <c r="B37">
-        <v>16.7512633245603</v>
-      </c>
-      <c r="C37">
-        <v>28.9133601927686</v>
-      </c>
-      <c r="D37">
-        <v>22.9829477488005</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38">
-        <v>90000</v>
-      </c>
-      <c r="B38">
-        <v>16.6033281494062</v>
-      </c>
-      <c r="C38">
-        <v>28.9133601927686</v>
-      </c>
-      <c r="D38">
-        <v>22.9829477488005</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39">
-        <v>95000</v>
-      </c>
-      <c r="B39">
-        <v>16.5266774326697</v>
-      </c>
-      <c r="C39">
-        <v>28.6935080892767</v>
-      </c>
-      <c r="D39">
-        <v>22.9829477488005</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40">
-        <v>100000</v>
-      </c>
-      <c r="B40">
-        <v>16.2116698633785</v>
-      </c>
-      <c r="C40">
-        <v>28.6935080892767</v>
-      </c>
-      <c r="D40">
-        <v>22.9829477488005</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1">
-      <c r="A58" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1">
-      <c r="A59" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1">
-      <c r="A60" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
-      <c r="A61" t="s">
-        <v>6</v>
-      </c>
-      <c r="B61" t="s">
-        <v>1</v>
-      </c>
-      <c r="C61" t="s">
-        <v>2</v>
-      </c>
-      <c r="D61" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
-      <c r="A62" t="s">
-        <v>7</v>
-      </c>
-      <c r="B62">
-        <v>100160</v>
-      </c>
-      <c r="C62">
-        <v>100160</v>
-      </c>
-      <c r="D62">
-        <v>100160</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4">
-      <c r="A63" t="s">
-        <v>8</v>
-      </c>
-      <c r="B63">
-        <v>16.202569012458</v>
-      </c>
-      <c r="C63">
-        <v>28.6935080892767</v>
-      </c>
-      <c r="D63">
-        <v>22.9829477488005</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
-      <c r="A64" t="s">
-        <v>9</v>
-      </c>
-      <c r="B64">
-        <v>16.202569012458</v>
-      </c>
-      <c r="C64">
-        <v>28.6935080892767</v>
-      </c>
-      <c r="D64">
-        <v>22.9829477488005</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4">
-      <c r="A65" t="s">
-        <v>10</v>
-      </c>
-      <c r="B65">
-        <v>15.8331394531904</v>
-      </c>
-      <c r="C65">
-        <v>25.8923274961828</v>
-      </c>
-      <c r="D65">
-        <v>23.2063653064899</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4">
-      <c r="A66" t="s">
-        <v>11</v>
-      </c>
-      <c r="B66">
-        <v>4.80491212021274</v>
-      </c>
-      <c r="C66">
-        <v>12.4799553886315</v>
-      </c>
-      <c r="D66">
-        <v>6.5896492979828</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:D66"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="A66" sqref="A61:A66"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="3"/>
-  <cols>
-    <col min="2" max="5" width="12.625"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2">
-        <v>5</v>
-      </c>
-      <c r="B2">
-        <v>85.7998731312975</v>
-      </c>
-      <c r="C2">
-        <v>85.7998731312975</v>
-      </c>
-      <c r="D2">
-        <v>85.7998731312975</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3">
-        <v>50</v>
-      </c>
-      <c r="B3">
-        <v>15.2693075295546</v>
-      </c>
-      <c r="C3">
-        <v>8.71195936543178</v>
-      </c>
-      <c r="D3">
-        <v>6.2229544343291</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4">
-        <v>100</v>
-      </c>
-      <c r="B4">
-        <v>3.84559200827463</v>
-      </c>
-      <c r="C4">
-        <v>1.93819667258339</v>
-      </c>
-      <c r="D4">
-        <v>2.85627970909732</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5">
-        <v>500</v>
-      </c>
-      <c r="B5">
-        <v>1.01722421267821</v>
-      </c>
-      <c r="C5">
-        <v>0.607947138065356</v>
-      </c>
-      <c r="D5">
-        <v>1.00381624018714</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6">
-        <v>1000</v>
-      </c>
-      <c r="B6">
-        <v>0.860677013763928</v>
-      </c>
-      <c r="C6">
-        <v>0.330796260469106</v>
-      </c>
-      <c r="D6">
-        <v>0.962725518147857</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7">
-        <v>1500</v>
-      </c>
-      <c r="B7">
-        <v>0.599923832612678</v>
-      </c>
-      <c r="C7">
-        <v>0.217075342932321</v>
-      </c>
-      <c r="D7">
-        <v>0.907495125090535</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8">
-        <v>2000</v>
-      </c>
-      <c r="B8">
-        <v>0.299012512494643</v>
-      </c>
-      <c r="C8">
-        <v>0.176278805969464</v>
-      </c>
-      <c r="D8">
-        <v>0.857100669395892</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9">
-        <v>2500</v>
-      </c>
-      <c r="B9">
-        <v>0.1902563427775</v>
-      </c>
-      <c r="C9">
-        <v>0.143313172849464</v>
-      </c>
-      <c r="D9">
-        <v>0.857094812253035</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10">
-        <v>3000</v>
-      </c>
-      <c r="B10">
-        <v>0.146797691834642</v>
-      </c>
-      <c r="C10">
-        <v>0.131471763272142</v>
-      </c>
-      <c r="D10">
-        <v>0.857094812253035</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11">
-        <v>3500</v>
-      </c>
-      <c r="B11">
-        <v>0.113819348474107</v>
-      </c>
-      <c r="C11">
-        <v>0.130071755237321</v>
-      </c>
-      <c r="D11">
-        <v>0.857094812253035</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12">
-        <v>4000</v>
-      </c>
-      <c r="B12">
-        <v>0.0877126966394643</v>
-      </c>
-      <c r="C12">
-        <v>0.124354426971964</v>
-      </c>
-      <c r="D12">
-        <v>0.857094812253035</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13">
-        <v>4500</v>
-      </c>
-      <c r="B13">
-        <v>0.0213259786021429</v>
-      </c>
-      <c r="C13">
-        <v>0.123237368257678</v>
-      </c>
-      <c r="D13">
-        <v>0.857094812253035</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14">
-        <v>5000</v>
-      </c>
-      <c r="B14">
-        <v>0.0213179390108929</v>
-      </c>
-      <c r="C14">
-        <v>0.119717317117678</v>
-      </c>
-      <c r="D14">
-        <v>0.857094812253035</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15">
-        <v>6000</v>
-      </c>
-      <c r="B15">
-        <v>0.0176724552794643</v>
-      </c>
-      <c r="C15">
-        <v>0.116301227843392</v>
-      </c>
-      <c r="D15">
-        <v>0.857094812253035</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16">
-        <v>7000</v>
-      </c>
-      <c r="B16">
-        <v>0.0115549973055357</v>
-      </c>
-      <c r="C16">
-        <v>0.112544188498035</v>
-      </c>
-      <c r="D16">
-        <v>0.857094812253035</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17">
-        <v>8000</v>
-      </c>
-      <c r="B17">
-        <v>0.00604981773410722</v>
-      </c>
-      <c r="C17">
-        <v>0.106945154938035</v>
-      </c>
-      <c r="D17">
-        <v>0.857094812253035</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18">
-        <v>9000</v>
-      </c>
-      <c r="B18">
-        <v>0.00548955943678578</v>
-      </c>
-      <c r="C18">
-        <v>0.10652477526125</v>
-      </c>
-      <c r="D18">
-        <v>0.857094812253035</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19">
-        <v>10000</v>
-      </c>
-      <c r="B19">
-        <v>0.00375737089160722</v>
-      </c>
-      <c r="C19">
-        <v>0.105922236186785</v>
-      </c>
-      <c r="D19">
-        <v>0.857094812253035</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20">
-        <v>12000</v>
-      </c>
-      <c r="B20">
-        <v>0.00205354522035718</v>
-      </c>
-      <c r="C20">
-        <v>0.104947584560535</v>
-      </c>
-      <c r="D20">
-        <v>0.857094812253035</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21">
-        <v>14000</v>
-      </c>
-      <c r="B21">
-        <v>0.00191995472607146</v>
-      </c>
-      <c r="C21">
-        <v>0.104924744560357</v>
-      </c>
-      <c r="D21">
-        <v>0.857094812253035</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22">
-        <v>16000</v>
-      </c>
-      <c r="B22">
-        <v>0.00135644607178575</v>
-      </c>
-      <c r="C22">
-        <v>0.103861854851428</v>
-      </c>
-      <c r="D22">
-        <v>0.857094812253035</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23">
-        <v>18000</v>
-      </c>
-      <c r="B23">
-        <v>0.00111036838339288</v>
-      </c>
-      <c r="C23">
-        <v>0.10380147111125</v>
-      </c>
-      <c r="D23">
-        <v>0.857094812253035</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24">
-        <v>20000</v>
-      </c>
-      <c r="B24">
-        <v>0.00093802352000003</v>
-      </c>
-      <c r="C24">
-        <v>0.103724304482678</v>
-      </c>
-      <c r="D24">
-        <v>0.857094812253035</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25">
-        <v>25000</v>
-      </c>
-      <c r="B25">
-        <v>0.000692824168214302</v>
-      </c>
-      <c r="C25">
-        <v>0.103328277868571</v>
-      </c>
-      <c r="D25">
-        <v>0.857094812253035</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26">
-        <v>30000</v>
-      </c>
-      <c r="B26">
-        <v>0.000584650753750016</v>
-      </c>
-      <c r="C26">
-        <v>0.10270160536875</v>
-      </c>
-      <c r="D26">
-        <v>0.857094812253035</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27">
-        <v>35000</v>
-      </c>
-      <c r="B27">
-        <v>0.000496944968214294</v>
-      </c>
-      <c r="C27">
-        <v>0.102469044380357</v>
-      </c>
-      <c r="D27">
-        <v>0.857094812253035</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28">
-        <v>40000</v>
-      </c>
-      <c r="B28">
-        <v>0.000249065176785718</v>
-      </c>
-      <c r="C28">
-        <v>0.102469044380357</v>
-      </c>
-      <c r="D28">
-        <v>0.857094812253035</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29">
-        <v>45000</v>
-      </c>
-      <c r="B29">
-        <v>0.000247311888392861</v>
-      </c>
-      <c r="C29">
-        <v>0.102350456000535</v>
-      </c>
-      <c r="D29">
-        <v>0.857094812253035</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30">
-        <v>50000</v>
-      </c>
-      <c r="B30">
-        <v>0.000240591880178573</v>
-      </c>
-      <c r="C30">
-        <v>0.102269566800714</v>
-      </c>
-      <c r="D30">
-        <v>0.857094812253035</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31">
-        <v>55000</v>
-      </c>
-      <c r="B31">
-        <v>0.000237892723392859</v>
-      </c>
-      <c r="C31">
-        <v>0.102242396420178</v>
-      </c>
-      <c r="D31">
-        <v>0.857094812253035</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32">
-        <v>60000</v>
-      </c>
-      <c r="B32">
-        <v>0.000237892723392859</v>
-      </c>
-      <c r="C32">
-        <v>0.102242396420178</v>
-      </c>
-      <c r="D32">
-        <v>0.857094812253035</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33">
-        <v>65000</v>
-      </c>
-      <c r="B33" s="1">
-        <v>5.79042058928649e-5</v>
-      </c>
-      <c r="C33">
-        <v>0.102198759600357</v>
-      </c>
-      <c r="D33">
-        <v>0.857094812253035</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34">
-        <v>70000</v>
-      </c>
-      <c r="B34" s="1">
-        <v>5.58184344642937e-5</v>
-      </c>
-      <c r="C34">
-        <v>0.102151119014464</v>
-      </c>
-      <c r="D34">
-        <v>0.857094812253035</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35">
-        <v>75000</v>
-      </c>
-      <c r="B35" s="1">
-        <v>5.49571085714372e-5</v>
-      </c>
-      <c r="C35">
-        <v>0.102147855585892</v>
-      </c>
-      <c r="D35">
-        <v>0.857094812253035</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36">
-        <v>80000</v>
-      </c>
-      <c r="B36" s="1">
-        <v>4.95095030357213e-5</v>
-      </c>
-      <c r="C36">
-        <v>0.10210475602875</v>
-      </c>
-      <c r="D36">
-        <v>0.857094812253035</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37">
-        <v>85000</v>
-      </c>
-      <c r="B37" s="1">
-        <v>4.36538491071499e-5</v>
-      </c>
-      <c r="C37">
-        <v>0.102056583962857</v>
-      </c>
-      <c r="D37">
-        <v>0.857094812253035</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38">
-        <v>90000</v>
-      </c>
-      <c r="B38" s="1">
-        <v>3.75606005357203e-5</v>
-      </c>
-      <c r="C38">
-        <v>0.102056583962857</v>
-      </c>
-      <c r="D38">
-        <v>0.857094812253035</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39">
-        <v>95000</v>
-      </c>
-      <c r="B39" s="1">
-        <v>3.20310833928628e-5</v>
-      </c>
-      <c r="C39">
-        <v>0.102041398265714</v>
-      </c>
-      <c r="D39">
-        <v>0.857094812253035</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40">
-        <v>100000</v>
-      </c>
-      <c r="B40" s="1">
-        <v>3.13435862500057e-5</v>
-      </c>
-      <c r="C40">
-        <v>0.102035383042678</v>
-      </c>
-      <c r="D40">
-        <v>0.857094812253035</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1">
-      <c r="A58" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1">
-      <c r="A59" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1">
-      <c r="A60" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
-      <c r="A61" t="s">
-        <v>6</v>
-      </c>
-      <c r="B61" t="s">
-        <v>1</v>
-      </c>
-      <c r="C61" t="s">
-        <v>2</v>
-      </c>
-      <c r="D61" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
-      <c r="A62" t="s">
-        <v>7</v>
-      </c>
-      <c r="B62">
-        <v>100022</v>
-      </c>
-      <c r="C62">
-        <v>100022</v>
-      </c>
-      <c r="D62">
-        <v>100022</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4">
-      <c r="A63" t="s">
-        <v>8</v>
-      </c>
-      <c r="B63" s="1">
-        <v>3.13435862500057e-5</v>
-      </c>
-      <c r="C63">
-        <v>0.102035383042678</v>
-      </c>
-      <c r="D63">
-        <v>0.857094812253035</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
-      <c r="A64" t="s">
-        <v>9</v>
-      </c>
-      <c r="B64" s="1">
-        <v>3.13435862500057e-5</v>
-      </c>
-      <c r="C64">
-        <v>0.102035383042678</v>
-      </c>
-      <c r="D64">
-        <v>0.857094812253035</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4">
-      <c r="A65" t="s">
-        <v>10</v>
-      </c>
-      <c r="B65" s="1">
-        <v>6.25390624999971e-6</v>
-      </c>
-      <c r="C65">
-        <v>0.000133999006250006</v>
-      </c>
-      <c r="D65">
-        <v>0.221193196099999</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4">
-      <c r="A66" t="s">
-        <v>11</v>
-      </c>
-      <c r="B66" s="1">
-        <v>4.51522884370941e-5</v>
-      </c>
-      <c r="C66">
-        <v>0.290102453102494</v>
-      </c>
-      <c r="D66">
-        <v>1.29031609592666</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:D66"/>
@@ -15436,6 +14112,1366 @@
         <v>5</v>
       </c>
       <c r="B2">
+        <v>222.161129866036</v>
+      </c>
+      <c r="C2">
+        <v>222.161129866036</v>
+      </c>
+      <c r="D2">
+        <v>222.161129866036</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>50</v>
+      </c>
+      <c r="B3">
+        <v>213.724838821676</v>
+      </c>
+      <c r="C3">
+        <v>213.724838821676</v>
+      </c>
+      <c r="D3">
+        <v>213.724838821676</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>100</v>
+      </c>
+      <c r="B4">
+        <v>211.685872228184</v>
+      </c>
+      <c r="C4">
+        <v>211.685872228184</v>
+      </c>
+      <c r="D4">
+        <v>211.685872228184</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>500</v>
+      </c>
+      <c r="B5">
+        <v>204.515499401897</v>
+      </c>
+      <c r="C5">
+        <v>149.449777442719</v>
+      </c>
+      <c r="D5">
+        <v>172.267340865898</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>1000</v>
+      </c>
+      <c r="B6">
+        <v>184.750695749215</v>
+      </c>
+      <c r="C6">
+        <v>80.663463015223</v>
+      </c>
+      <c r="D6">
+        <v>98.2744348587591</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>1500</v>
+      </c>
+      <c r="B7">
+        <v>164.465094624622</v>
+      </c>
+      <c r="C7">
+        <v>55.5958350050346</v>
+      </c>
+      <c r="D7">
+        <v>60.9599290430378</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>2000</v>
+      </c>
+      <c r="B8">
+        <v>138.575992131484</v>
+      </c>
+      <c r="C8">
+        <v>40.7587350167379</v>
+      </c>
+      <c r="D8">
+        <v>35.0600721878919</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <v>2500</v>
+      </c>
+      <c r="B9">
+        <v>119.922287280342</v>
+      </c>
+      <c r="C9">
+        <v>37.2310478129347</v>
+      </c>
+      <c r="D9">
+        <v>28.4665142296936</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <v>3000</v>
+      </c>
+      <c r="B10">
+        <v>97.9407311838834</v>
+      </c>
+      <c r="C10">
+        <v>35.8153540633938</v>
+      </c>
+      <c r="D10">
+        <v>23.894178092588</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11">
+        <v>3500</v>
+      </c>
+      <c r="B11">
+        <v>87.7959498851028</v>
+      </c>
+      <c r="C11">
+        <v>34.5709190485729</v>
+      </c>
+      <c r="D11">
+        <v>23.6504376355184</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12">
+        <v>4000</v>
+      </c>
+      <c r="B12">
+        <v>73.4884609402364</v>
+      </c>
+      <c r="C12">
+        <v>33.1898609925408</v>
+      </c>
+      <c r="D12">
+        <v>23.0969328230867</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13">
+        <v>4500</v>
+      </c>
+      <c r="B13">
+        <v>65.0233974426678</v>
+      </c>
+      <c r="C13">
+        <v>32.8577532110956</v>
+      </c>
+      <c r="D13">
+        <v>23.006663331618</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14">
+        <v>5000</v>
+      </c>
+      <c r="B14">
+        <v>57.3025687064767</v>
+      </c>
+      <c r="C14">
+        <v>32.4111113053343</v>
+      </c>
+      <c r="D14">
+        <v>22.9883156411679</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15">
+        <v>6000</v>
+      </c>
+      <c r="B15">
+        <v>46.1653576900982</v>
+      </c>
+      <c r="C15">
+        <v>32.1101767449222</v>
+      </c>
+      <c r="D15">
+        <v>22.9830527697315</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16">
+        <v>7000</v>
+      </c>
+      <c r="B16">
+        <v>38.1521149027307</v>
+      </c>
+      <c r="C16">
+        <v>31.8996822561839</v>
+      </c>
+      <c r="D16">
+        <v>22.9830275566717</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17">
+        <v>8000</v>
+      </c>
+      <c r="B17">
+        <v>32.2688119830113</v>
+      </c>
+      <c r="C17">
+        <v>31.5867922309758</v>
+      </c>
+      <c r="D17">
+        <v>22.982949079113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18">
+        <v>9000</v>
+      </c>
+      <c r="B18">
+        <v>27.7597428378178</v>
+      </c>
+      <c r="C18">
+        <v>31.133469335833</v>
+      </c>
+      <c r="D18">
+        <v>22.9829477488005</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19">
+        <v>10000</v>
+      </c>
+      <c r="B19">
+        <v>24.9656141777948</v>
+      </c>
+      <c r="C19">
+        <v>31.133469335833</v>
+      </c>
+      <c r="D19">
+        <v>22.9829477488005</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20">
+        <v>12000</v>
+      </c>
+      <c r="B20">
+        <v>21.9647140986413</v>
+      </c>
+      <c r="C20">
+        <v>31.0993392553022</v>
+      </c>
+      <c r="D20">
+        <v>22.9829477488005</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21">
+        <v>14000</v>
+      </c>
+      <c r="B21">
+        <v>20.7589879315573</v>
+      </c>
+      <c r="C21">
+        <v>30.963941267577</v>
+      </c>
+      <c r="D21">
+        <v>22.9829477488005</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22">
+        <v>16000</v>
+      </c>
+      <c r="B22">
+        <v>20.320069303179</v>
+      </c>
+      <c r="C22">
+        <v>30.8132192429305</v>
+      </c>
+      <c r="D22">
+        <v>22.9829477488005</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23">
+        <v>18000</v>
+      </c>
+      <c r="B23">
+        <v>20.1162173990172</v>
+      </c>
+      <c r="C23">
+        <v>30.8132192429305</v>
+      </c>
+      <c r="D23">
+        <v>22.9829477488005</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24">
+        <v>20000</v>
+      </c>
+      <c r="B24">
+        <v>19.9195687017421</v>
+      </c>
+      <c r="C24">
+        <v>30.444225290351</v>
+      </c>
+      <c r="D24">
+        <v>22.9829477488005</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25">
+        <v>25000</v>
+      </c>
+      <c r="B25">
+        <v>19.8540728752238</v>
+      </c>
+      <c r="C25">
+        <v>30.444225290351</v>
+      </c>
+      <c r="D25">
+        <v>22.9829477488005</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26">
+        <v>30000</v>
+      </c>
+      <c r="B26">
+        <v>19.8428338080667</v>
+      </c>
+      <c r="C26">
+        <v>30.2103916561594</v>
+      </c>
+      <c r="D26">
+        <v>22.9829477488005</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27">
+        <v>35000</v>
+      </c>
+      <c r="B27">
+        <v>19.8141065956705</v>
+      </c>
+      <c r="C27">
+        <v>30.2103916561594</v>
+      </c>
+      <c r="D27">
+        <v>22.9829477488005</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28">
+        <v>40000</v>
+      </c>
+      <c r="B28">
+        <v>19.7453584808793</v>
+      </c>
+      <c r="C28">
+        <v>29.8394041069721</v>
+      </c>
+      <c r="D28">
+        <v>22.9829477488005</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29">
+        <v>45000</v>
+      </c>
+      <c r="B29">
+        <v>18.983288489317</v>
+      </c>
+      <c r="C29">
+        <v>28.9133601927686</v>
+      </c>
+      <c r="D29">
+        <v>22.9829477488005</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30">
+        <v>50000</v>
+      </c>
+      <c r="B30">
+        <v>18.4746244124938</v>
+      </c>
+      <c r="C30">
+        <v>28.9133601927686</v>
+      </c>
+      <c r="D30">
+        <v>22.9829477488005</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31">
+        <v>55000</v>
+      </c>
+      <c r="B31">
+        <v>17.9927469397173</v>
+      </c>
+      <c r="C31">
+        <v>28.9133601927686</v>
+      </c>
+      <c r="D31">
+        <v>22.9829477488005</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32">
+        <v>60000</v>
+      </c>
+      <c r="B32">
+        <v>17.695699611482</v>
+      </c>
+      <c r="C32">
+        <v>28.9133601927686</v>
+      </c>
+      <c r="D32">
+        <v>22.9829477488005</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33">
+        <v>65000</v>
+      </c>
+      <c r="B33">
+        <v>17.4420595328849</v>
+      </c>
+      <c r="C33">
+        <v>28.9133601927686</v>
+      </c>
+      <c r="D33">
+        <v>22.9829477488005</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34">
+        <v>70000</v>
+      </c>
+      <c r="B34">
+        <v>17.2169735857428</v>
+      </c>
+      <c r="C34">
+        <v>28.9133601927686</v>
+      </c>
+      <c r="D34">
+        <v>22.9829477488005</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35">
+        <v>75000</v>
+      </c>
+      <c r="B35">
+        <v>16.9728026776156</v>
+      </c>
+      <c r="C35">
+        <v>28.9133601927686</v>
+      </c>
+      <c r="D35">
+        <v>22.9829477488005</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36">
+        <v>80000</v>
+      </c>
+      <c r="B36">
+        <v>16.8804150028953</v>
+      </c>
+      <c r="C36">
+        <v>28.9133601927686</v>
+      </c>
+      <c r="D36">
+        <v>22.9829477488005</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37">
+        <v>85000</v>
+      </c>
+      <c r="B37">
+        <v>16.7512633245603</v>
+      </c>
+      <c r="C37">
+        <v>28.9133601927686</v>
+      </c>
+      <c r="D37">
+        <v>22.9829477488005</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38">
+        <v>90000</v>
+      </c>
+      <c r="B38">
+        <v>16.6033281494062</v>
+      </c>
+      <c r="C38">
+        <v>28.9133601927686</v>
+      </c>
+      <c r="D38">
+        <v>22.9829477488005</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39">
+        <v>95000</v>
+      </c>
+      <c r="B39">
+        <v>16.5266774326697</v>
+      </c>
+      <c r="C39">
+        <v>28.6935080892767</v>
+      </c>
+      <c r="D39">
+        <v>22.9829477488005</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40">
+        <v>100000</v>
+      </c>
+      <c r="B40">
+        <v>16.2116698633785</v>
+      </c>
+      <c r="C40">
+        <v>28.6935080892767</v>
+      </c>
+      <c r="D40">
+        <v>22.9829477488005</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" t="s">
+        <v>6</v>
+      </c>
+      <c r="B61" t="s">
+        <v>1</v>
+      </c>
+      <c r="C61" t="s">
+        <v>2</v>
+      </c>
+      <c r="D61" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" t="s">
+        <v>7</v>
+      </c>
+      <c r="B62">
+        <v>100160</v>
+      </c>
+      <c r="C62">
+        <v>100160</v>
+      </c>
+      <c r="D62">
+        <v>100160</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" t="s">
+        <v>8</v>
+      </c>
+      <c r="B63">
+        <v>16.202569012458</v>
+      </c>
+      <c r="C63">
+        <v>28.6935080892767</v>
+      </c>
+      <c r="D63">
+        <v>22.9829477488005</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" t="s">
+        <v>9</v>
+      </c>
+      <c r="B64">
+        <v>16.202569012458</v>
+      </c>
+      <c r="C64">
+        <v>28.6935080892767</v>
+      </c>
+      <c r="D64">
+        <v>22.9829477488005</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" t="s">
+        <v>10</v>
+      </c>
+      <c r="B65">
+        <v>15.8331394531904</v>
+      </c>
+      <c r="C65">
+        <v>25.8923274961828</v>
+      </c>
+      <c r="D65">
+        <v>23.2063653064899</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" t="s">
+        <v>11</v>
+      </c>
+      <c r="B66">
+        <v>4.80491212021274</v>
+      </c>
+      <c r="C66">
+        <v>12.4799553886315</v>
+      </c>
+      <c r="D66">
+        <v>6.5896492979828</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D66"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="J50" sqref="J50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="3"/>
+  <cols>
+    <col min="2" max="5" width="12.625"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>85.7998731312975</v>
+      </c>
+      <c r="C2">
+        <v>85.7998731312975</v>
+      </c>
+      <c r="D2">
+        <v>85.7998731312975</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>50</v>
+      </c>
+      <c r="B3">
+        <v>15.2693075295546</v>
+      </c>
+      <c r="C3">
+        <v>8.71195936543178</v>
+      </c>
+      <c r="D3">
+        <v>6.2229544343291</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>100</v>
+      </c>
+      <c r="B4">
+        <v>3.84559200827463</v>
+      </c>
+      <c r="C4">
+        <v>1.93819667258339</v>
+      </c>
+      <c r="D4">
+        <v>2.85627970909732</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>500</v>
+      </c>
+      <c r="B5">
+        <v>1.01722421267821</v>
+      </c>
+      <c r="C5">
+        <v>0.607947138065356</v>
+      </c>
+      <c r="D5">
+        <v>1.00381624018714</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>1000</v>
+      </c>
+      <c r="B6">
+        <v>0.860677013763928</v>
+      </c>
+      <c r="C6">
+        <v>0.330796260469106</v>
+      </c>
+      <c r="D6">
+        <v>0.962725518147857</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>1500</v>
+      </c>
+      <c r="B7">
+        <v>0.599923832612678</v>
+      </c>
+      <c r="C7">
+        <v>0.217075342932321</v>
+      </c>
+      <c r="D7">
+        <v>0.907495125090535</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>2000</v>
+      </c>
+      <c r="B8">
+        <v>0.299012512494643</v>
+      </c>
+      <c r="C8">
+        <v>0.176278805969464</v>
+      </c>
+      <c r="D8">
+        <v>0.857100669395892</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <v>2500</v>
+      </c>
+      <c r="B9">
+        <v>0.1902563427775</v>
+      </c>
+      <c r="C9">
+        <v>0.143313172849464</v>
+      </c>
+      <c r="D9">
+        <v>0.857094812253035</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <v>3000</v>
+      </c>
+      <c r="B10">
+        <v>0.146797691834642</v>
+      </c>
+      <c r="C10">
+        <v>0.131471763272142</v>
+      </c>
+      <c r="D10">
+        <v>0.857094812253035</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11">
+        <v>3500</v>
+      </c>
+      <c r="B11">
+        <v>0.113819348474107</v>
+      </c>
+      <c r="C11">
+        <v>0.130071755237321</v>
+      </c>
+      <c r="D11">
+        <v>0.857094812253035</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12">
+        <v>4000</v>
+      </c>
+      <c r="B12">
+        <v>0.0877126966394643</v>
+      </c>
+      <c r="C12">
+        <v>0.124354426971964</v>
+      </c>
+      <c r="D12">
+        <v>0.857094812253035</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13">
+        <v>4500</v>
+      </c>
+      <c r="B13">
+        <v>0.0213259786021429</v>
+      </c>
+      <c r="C13">
+        <v>0.123237368257678</v>
+      </c>
+      <c r="D13">
+        <v>0.857094812253035</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14">
+        <v>5000</v>
+      </c>
+      <c r="B14">
+        <v>0.0213179390108929</v>
+      </c>
+      <c r="C14">
+        <v>0.119717317117678</v>
+      </c>
+      <c r="D14">
+        <v>0.857094812253035</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15">
+        <v>6000</v>
+      </c>
+      <c r="B15">
+        <v>0.0176724552794643</v>
+      </c>
+      <c r="C15">
+        <v>0.116301227843392</v>
+      </c>
+      <c r="D15">
+        <v>0.857094812253035</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16">
+        <v>7000</v>
+      </c>
+      <c r="B16">
+        <v>0.0115549973055357</v>
+      </c>
+      <c r="C16">
+        <v>0.112544188498035</v>
+      </c>
+      <c r="D16">
+        <v>0.857094812253035</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17">
+        <v>8000</v>
+      </c>
+      <c r="B17">
+        <v>0.00604981773410722</v>
+      </c>
+      <c r="C17">
+        <v>0.106945154938035</v>
+      </c>
+      <c r="D17">
+        <v>0.857094812253035</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18">
+        <v>9000</v>
+      </c>
+      <c r="B18">
+        <v>0.00548955943678578</v>
+      </c>
+      <c r="C18">
+        <v>0.10652477526125</v>
+      </c>
+      <c r="D18">
+        <v>0.857094812253035</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19">
+        <v>10000</v>
+      </c>
+      <c r="B19">
+        <v>0.00375737089160722</v>
+      </c>
+      <c r="C19">
+        <v>0.105922236186785</v>
+      </c>
+      <c r="D19">
+        <v>0.857094812253035</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20">
+        <v>12000</v>
+      </c>
+      <c r="B20">
+        <v>0.00205354522035718</v>
+      </c>
+      <c r="C20">
+        <v>0.104947584560535</v>
+      </c>
+      <c r="D20">
+        <v>0.857094812253035</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21">
+        <v>14000</v>
+      </c>
+      <c r="B21">
+        <v>0.00191995472607146</v>
+      </c>
+      <c r="C21">
+        <v>0.104924744560357</v>
+      </c>
+      <c r="D21">
+        <v>0.857094812253035</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22">
+        <v>16000</v>
+      </c>
+      <c r="B22">
+        <v>0.00135644607178575</v>
+      </c>
+      <c r="C22">
+        <v>0.103861854851428</v>
+      </c>
+      <c r="D22">
+        <v>0.857094812253035</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23">
+        <v>18000</v>
+      </c>
+      <c r="B23">
+        <v>0.00111036838339288</v>
+      </c>
+      <c r="C23">
+        <v>0.10380147111125</v>
+      </c>
+      <c r="D23">
+        <v>0.857094812253035</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24">
+        <v>20000</v>
+      </c>
+      <c r="B24">
+        <v>0.00093802352000003</v>
+      </c>
+      <c r="C24">
+        <v>0.103724304482678</v>
+      </c>
+      <c r="D24">
+        <v>0.857094812253035</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25">
+        <v>25000</v>
+      </c>
+      <c r="B25">
+        <v>0.000692824168214302</v>
+      </c>
+      <c r="C25">
+        <v>0.103328277868571</v>
+      </c>
+      <c r="D25">
+        <v>0.857094812253035</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26">
+        <v>30000</v>
+      </c>
+      <c r="B26">
+        <v>0.000584650753750016</v>
+      </c>
+      <c r="C26">
+        <v>0.10270160536875</v>
+      </c>
+      <c r="D26">
+        <v>0.857094812253035</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27">
+        <v>35000</v>
+      </c>
+      <c r="B27">
+        <v>0.000496944968214294</v>
+      </c>
+      <c r="C27">
+        <v>0.102469044380357</v>
+      </c>
+      <c r="D27">
+        <v>0.857094812253035</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28">
+        <v>40000</v>
+      </c>
+      <c r="B28">
+        <v>0.000249065176785718</v>
+      </c>
+      <c r="C28">
+        <v>0.102469044380357</v>
+      </c>
+      <c r="D28">
+        <v>0.857094812253035</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29">
+        <v>45000</v>
+      </c>
+      <c r="B29">
+        <v>0.000247311888392861</v>
+      </c>
+      <c r="C29">
+        <v>0.102350456000535</v>
+      </c>
+      <c r="D29">
+        <v>0.857094812253035</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30">
+        <v>50000</v>
+      </c>
+      <c r="B30">
+        <v>0.000240591880178573</v>
+      </c>
+      <c r="C30">
+        <v>0.102269566800714</v>
+      </c>
+      <c r="D30">
+        <v>0.857094812253035</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31">
+        <v>55000</v>
+      </c>
+      <c r="B31">
+        <v>0.000237892723392859</v>
+      </c>
+      <c r="C31">
+        <v>0.102242396420178</v>
+      </c>
+      <c r="D31">
+        <v>0.857094812253035</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32">
+        <v>60000</v>
+      </c>
+      <c r="B32">
+        <v>0.000237892723392859</v>
+      </c>
+      <c r="C32">
+        <v>0.102242396420178</v>
+      </c>
+      <c r="D32">
+        <v>0.857094812253035</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33">
+        <v>65000</v>
+      </c>
+      <c r="B33" s="1">
+        <v>5.79042058928649e-5</v>
+      </c>
+      <c r="C33">
+        <v>0.102198759600357</v>
+      </c>
+      <c r="D33">
+        <v>0.857094812253035</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34">
+        <v>70000</v>
+      </c>
+      <c r="B34" s="1">
+        <v>5.58184344642937e-5</v>
+      </c>
+      <c r="C34">
+        <v>0.102151119014464</v>
+      </c>
+      <c r="D34">
+        <v>0.857094812253035</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35">
+        <v>75000</v>
+      </c>
+      <c r="B35" s="1">
+        <v>5.49571085714372e-5</v>
+      </c>
+      <c r="C35">
+        <v>0.102147855585892</v>
+      </c>
+      <c r="D35">
+        <v>0.857094812253035</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36">
+        <v>80000</v>
+      </c>
+      <c r="B36" s="1">
+        <v>4.95095030357213e-5</v>
+      </c>
+      <c r="C36">
+        <v>0.10210475602875</v>
+      </c>
+      <c r="D36">
+        <v>0.857094812253035</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37">
+        <v>85000</v>
+      </c>
+      <c r="B37" s="1">
+        <v>4.36538491071499e-5</v>
+      </c>
+      <c r="C37">
+        <v>0.102056583962857</v>
+      </c>
+      <c r="D37">
+        <v>0.857094812253035</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38">
+        <v>90000</v>
+      </c>
+      <c r="B38" s="1">
+        <v>3.75606005357203e-5</v>
+      </c>
+      <c r="C38">
+        <v>0.102056583962857</v>
+      </c>
+      <c r="D38">
+        <v>0.857094812253035</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39">
+        <v>95000</v>
+      </c>
+      <c r="B39" s="1">
+        <v>3.20310833928628e-5</v>
+      </c>
+      <c r="C39">
+        <v>0.102041398265714</v>
+      </c>
+      <c r="D39">
+        <v>0.857094812253035</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40">
+        <v>100000</v>
+      </c>
+      <c r="B40" s="1">
+        <v>3.13435862500057e-5</v>
+      </c>
+      <c r="C40">
+        <v>0.102035383042678</v>
+      </c>
+      <c r="D40">
+        <v>0.857094812253035</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" t="s">
+        <v>6</v>
+      </c>
+      <c r="B61" t="s">
+        <v>1</v>
+      </c>
+      <c r="C61" t="s">
+        <v>2</v>
+      </c>
+      <c r="D61" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" t="s">
+        <v>7</v>
+      </c>
+      <c r="B62">
+        <v>100022</v>
+      </c>
+      <c r="C62">
+        <v>100022</v>
+      </c>
+      <c r="D62">
+        <v>100022</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" t="s">
+        <v>8</v>
+      </c>
+      <c r="B63" s="1">
+        <v>3.13435862500057e-5</v>
+      </c>
+      <c r="C63">
+        <v>0.102035383042678</v>
+      </c>
+      <c r="D63">
+        <v>0.857094812253035</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" t="s">
+        <v>9</v>
+      </c>
+      <c r="B64" s="1">
+        <v>3.13435862500057e-5</v>
+      </c>
+      <c r="C64">
+        <v>0.102035383042678</v>
+      </c>
+      <c r="D64">
+        <v>0.857094812253035</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" t="s">
+        <v>10</v>
+      </c>
+      <c r="B65" s="1">
+        <v>6.25390624999971e-6</v>
+      </c>
+      <c r="C65">
+        <v>0.000133999006250006</v>
+      </c>
+      <c r="D65">
+        <v>0.221193196099999</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" t="s">
+        <v>11</v>
+      </c>
+      <c r="B66" s="1">
+        <v>4.51522884370941e-5</v>
+      </c>
+      <c r="C66">
+        <v>0.290102453102494</v>
+      </c>
+      <c r="D66">
+        <v>1.29031609592666</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D66"/>
+  <sheetViews>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D68" sqref="D68"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="3"/>
+  <cols>
+    <col min="2" max="5" width="12.625"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>5</v>
+      </c>
+      <c r="B2">
         <v>4139.84127120515</v>
       </c>
       <c r="C2">
@@ -16088,8 +16124,8 @@
   <sheetPr/>
   <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61:A66"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="3"/>
@@ -16768,8 +16804,8 @@
   <sheetPr/>
   <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C66" sqref="C62:C66"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="3"/>

</xml_diff>